<commit_message>
Memoria del Proyecto actualizada
</commit_message>
<xml_diff>
--- a/0-varios/Acciones-para-links.xlsx
+++ b/0-varios/Acciones-para-links.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Documents\1. Proyectos Web\ELC-Peliculas\0-varios\1. Backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\Documents\1. Proyectos Web\ELC-Peliculas\0-varios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>RUD</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>inactivar+m</t>
-  </si>
-  <si>
-    <t>inactivado+m</t>
   </si>
   <si>
     <t>Q</t>
@@ -114,13 +111,16 @@
     <t>Deshacer</t>
   </si>
   <si>
-    <t>ajenos3</t>
-  </si>
-  <si>
     <t>en original</t>
   </si>
   <si>
     <t>en edicion</t>
+  </si>
+  <si>
+    <t>inactivo</t>
+  </si>
+  <si>
+    <t>ajenos_x_3</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -386,15 +386,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
@@ -404,9 +395,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -431,33 +419,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -465,9 +438,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -484,19 +454,106 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -508,106 +565,31 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -633,13 +615,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>163424</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -933,291 +915,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
-      <c r="B1" s="42"/>
+      <c r="B1" s="30"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="8" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="50"/>
+      <c r="F2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="32"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="52"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="34"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+    </row>
+    <row r="5" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="53"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="28"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="70">
+        <v>3</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="46"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="71"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="38"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="40"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="66"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="73"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="38"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="67"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="66"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="73"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="43"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="67"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="57"/>
+      <c r="B12" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="9"/>
-    </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="63" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="59" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="78" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="80" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="26" t="s">
+      <c r="C12" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="46"/>
+      <c r="F12" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="58"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="38"/>
+      <c r="F13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-    </row>
-    <row r="5" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="77"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="67" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="38"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>3</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="69"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="73" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="51"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="43"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="43"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="57"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
-      <c r="B13" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="49"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E11"/>
+    <mergeCell ref="D12:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>